<commit_message>
updated code access pattern analysis
</commit_message>
<xml_diff>
--- a/shared_ptp_new.xlsx
+++ b/shared_ptp_new.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="439" documentId="8_{7156C829-7D86-4EAD-B166-CA96C90DE1E5}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{589D4181-61AB-49AF-9775-D64BF2BE1A04}"/>
+  <xr:revisionPtr revIDLastSave="514" documentId="8_{7156C829-7D86-4EAD-B166-CA96C90DE1E5}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{518CB9FD-BFAC-43EA-B6A4-A0E6B74A8CFA}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="125">
   <si>
     <t>empty main function</t>
   </si>
@@ -354,10 +354,52 @@
     <t>total # of 4KB pages</t>
   </si>
   <si>
-    <t># of contiguous 4KB pages accessed</t>
-  </si>
-  <si>
-    <t>frequency</t>
+    <t>proc -v RES</t>
+  </si>
+  <si>
+    <t>clang</t>
+  </si>
+  <si>
+    <t>postgres</t>
+  </si>
+  <si>
+    <t>SPECjvm</t>
+  </si>
+  <si>
+    <t>derby</t>
+  </si>
+  <si>
+    <t>/usr/local/openjdk8/jre/lib/amd64/libjava.so</t>
+  </si>
+  <si>
+    <t>/usr/local/openjdk8/jre/lib/amd64/libverify.so</t>
+  </si>
+  <si>
+    <t>/usr/local/openjdk8/jre/lib/amd64/libzip.so</t>
+  </si>
+  <si>
+    <t>/usr/local/openjdk8/bin/java</t>
+  </si>
+  <si>
+    <t>/usr/local/openjdk8/jre/lib/amd64/libnet.so</t>
+  </si>
+  <si>
+    <t>/usr/local/openjdk8/jre/lib/amd64/libnio.so</t>
+  </si>
+  <si>
+    <t>/usr/local/openjdk8/jre/lib/amd64/server/libjvm.so</t>
+  </si>
+  <si>
+    <t>/usr/local/openjdk8/lib/amd64/jli/libjli.so</t>
+  </si>
+  <si>
+    <t>compiler.compiler</t>
+  </si>
+  <si>
+    <t>serial</t>
+  </si>
+  <si>
+    <t>xml.transform</t>
   </si>
 </sst>
 </file>
@@ -367,7 +409,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -408,6 +450,14 @@
     <font>
       <sz val="11"/>
       <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -478,7 +528,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -534,6 +584,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -550,2183 +603,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>postgres binary </a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t>access pattern</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:numRef>
-              <c:f>'app code access pattern'!$A$24:$A$38</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>41</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'app code access pattern'!$B$24:$B$38</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
-                <c:pt idx="0">
-                  <c:v>45</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-84EF-4B7D-B5C3-27D07296D482}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="656348896"/>
-        <c:axId val="656349880"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="656348896"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>frequency</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="656349880"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="656349880"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>#</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> of contiguous 4KB pages accessed</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="656348896"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>clang binary access</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> pattern</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:numRef>
-              <c:f>'app code access pattern'!$A$43:$A$61</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>23</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'app code access pattern'!$B$43:$B$61</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
-                <c:pt idx="0">
-                  <c:v>254</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>132</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>29</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-2CC8-4998-B37B-D5D5C8285433}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="656353816"/>
-        <c:axId val="656351848"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="656353816"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>frequency</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="656351848"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="656351848"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>#</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> of contiguous 4KB pages accessed</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="656353816"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1235868</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>278606</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>602456</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>126206</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E7AE85D1-D885-4AF5-9281-F333237BDC2E}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1140618</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>150018</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>395288</xdr:colOff>
-      <xdr:row>60</xdr:row>
-      <xdr:rowOff>57149</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9913D73C-51F4-4E99-857A-C193428D5FCF}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4957,7 +2833,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -5103,545 +2979,1064 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F2B83D2-17B5-4C3C-AEB8-7A16A8B053BB}">
-  <dimension ref="A1:J61"/>
+  <dimension ref="A1:J106"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="18.53125" customWidth="1"/>
+    <col min="1" max="1" width="45.53125" customWidth="1"/>
     <col min="2" max="2" width="20.86328125" customWidth="1"/>
     <col min="3" max="3" width="18.46484375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A1" s="30" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A2" s="28" t="s">
         <v>88</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B2" s="28" t="s">
         <v>90</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C2" s="28" t="s">
         <v>108</v>
       </c>
-      <c r="D1" s="28"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A2" s="23" t="s">
+      <c r="D2" s="29" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A3" s="28" t="s">
         <v>89</v>
       </c>
-      <c r="B2" s="23">
-        <v>1445</v>
-      </c>
-      <c r="C2" s="23">
+      <c r="B3" s="28">
+        <v>1872</v>
+      </c>
+      <c r="C3" s="28">
         <v>10700</v>
       </c>
-      <c r="D2" s="28"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A3" s="23"/>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
       <c r="D3" s="28"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="28"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A5" s="28"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+    </row>
+    <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A6" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="B6" s="28"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A7" s="28" t="s">
+        <v>88</v>
+      </c>
+      <c r="B7" s="28" t="s">
+        <v>90</v>
+      </c>
+      <c r="C7" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="D7" s="29" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
         <v>91</v>
       </c>
-      <c r="B4" s="23">
-        <v>374</v>
-      </c>
-      <c r="C4" s="23">
+      <c r="B8">
+        <v>524</v>
+      </c>
+      <c r="C8">
         <v>1506</v>
       </c>
-      <c r="D4" s="28"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A5" s="23" t="s">
+      <c r="D8" s="28">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
         <v>92</v>
       </c>
-      <c r="B5" s="23">
+      <c r="B9">
         <v>9</v>
       </c>
-      <c r="C5" s="23">
+      <c r="C9">
         <v>576</v>
       </c>
-      <c r="D5" s="28"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A6" s="23" t="s">
+      <c r="D9" s="28"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
         <v>93</v>
       </c>
-      <c r="B6" s="23">
+      <c r="B10">
         <v>0</v>
       </c>
-      <c r="C6" s="23">
+      <c r="C10">
         <v>394</v>
       </c>
-      <c r="D6" s="28"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A7" s="23" t="s">
+      <c r="D10" s="28"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
         <v>94</v>
       </c>
-      <c r="B7" s="23">
+      <c r="B11">
         <v>0</v>
       </c>
-      <c r="C7" s="23">
+      <c r="C11">
         <v>27</v>
       </c>
-      <c r="D7" s="28"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A8" s="23" t="s">
+      <c r="D11" s="28"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
         <v>95</v>
       </c>
-      <c r="B8" s="23">
+      <c r="B12">
         <v>0</v>
       </c>
-      <c r="C8" s="23">
+      <c r="C12">
         <v>23</v>
       </c>
-      <c r="D8" s="28"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A9" s="23" t="s">
+      <c r="D12" s="28"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
         <v>96</v>
       </c>
-      <c r="B9" s="23">
+      <c r="B13">
         <v>0</v>
       </c>
-      <c r="C9" s="23">
+      <c r="C13">
         <v>42</v>
       </c>
-      <c r="D9" s="28"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A10" s="23" t="s">
+      <c r="D13" s="28"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
         <v>97</v>
       </c>
-      <c r="B10" s="23">
+      <c r="B14">
+        <v>4</v>
+      </c>
+      <c r="C14">
+        <v>102</v>
+      </c>
+      <c r="D14" s="28"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>98</v>
+      </c>
+      <c r="B15">
         <v>0</v>
       </c>
-      <c r="C10" s="23">
+      <c r="C15">
+        <v>183</v>
+      </c>
+      <c r="D15" s="28"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>99</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>439</v>
+      </c>
+      <c r="D16" s="28"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>100</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>25</v>
+      </c>
+      <c r="D17" s="28"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
+        <v>101</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>14</v>
+      </c>
+      <c r="D18" s="28"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
         <v>102</v>
       </c>
-      <c r="D10" s="28"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A11" s="23" t="s">
-        <v>98</v>
-      </c>
-      <c r="B11" s="23">
-        <v>0</v>
-      </c>
-      <c r="C11" s="23">
-        <v>183</v>
-      </c>
-      <c r="D11" s="28"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A12" s="23" t="s">
-        <v>99</v>
-      </c>
-      <c r="B12" s="23">
-        <v>0</v>
-      </c>
-      <c r="C12" s="23">
-        <v>439</v>
-      </c>
-      <c r="D12" s="28"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A13" s="23" t="s">
-        <v>100</v>
-      </c>
-      <c r="B13" s="23">
-        <v>0</v>
-      </c>
-      <c r="C13" s="23">
-        <v>25</v>
-      </c>
-      <c r="D13" s="28"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A14" s="23" t="s">
-        <v>101</v>
-      </c>
-      <c r="B14" s="23">
-        <v>0</v>
-      </c>
-      <c r="C14" s="23">
-        <v>14</v>
-      </c>
-      <c r="D14" s="28"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A15" s="23" t="s">
-        <v>102</v>
-      </c>
-      <c r="B15" s="23">
-        <v>2</v>
-      </c>
-      <c r="C15" s="23">
+      <c r="B19">
+        <v>4</v>
+      </c>
+      <c r="C19">
         <v>716</v>
       </c>
-      <c r="D15" s="28"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A16" s="23" t="s">
+      <c r="D19" s="28"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
         <v>103</v>
       </c>
-      <c r="B16" s="23">
-        <v>0</v>
-      </c>
-      <c r="C16" s="23">
+      <c r="B20">
+        <v>26</v>
+      </c>
+      <c r="C20">
         <v>40</v>
       </c>
-      <c r="D16" s="28"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A17" s="23" t="s">
+      <c r="D20" s="28"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
         <v>104</v>
       </c>
-      <c r="B17" s="23">
+      <c r="B21">
         <v>5</v>
       </c>
-      <c r="C17" s="23">
+      <c r="C21">
         <v>565</v>
       </c>
-      <c r="D17" s="28"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A18" s="23" t="s">
-        <v>105</v>
-      </c>
-      <c r="B18" s="23">
-        <v>0</v>
-      </c>
-      <c r="C18" s="23">
-        <v>31</v>
-      </c>
-      <c r="D18" s="28"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A19" s="23" t="s">
-        <v>106</v>
-      </c>
-      <c r="B19" s="23">
-        <v>0</v>
-      </c>
-      <c r="C19" s="23">
-        <v>10</v>
-      </c>
-      <c r="D19" s="28"/>
+      <c r="D21" s="28"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A23" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="B23" t="s">
-        <v>110</v>
-      </c>
-      <c r="J23" t="s">
+        <v>105</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>31</v>
+      </c>
+      <c r="D22" s="28"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>106</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>10</v>
+      </c>
+      <c r="D23" s="28"/>
+    </row>
+    <row r="25" spans="1:10" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A25" s="30" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A26" s="8" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A27" s="28" t="s">
+        <v>88</v>
+      </c>
+      <c r="B27" s="28" t="s">
+        <v>90</v>
+      </c>
+      <c r="C27" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="D27" s="29"/>
+      <c r="J27" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A24">
-        <v>1</v>
-      </c>
-      <c r="B24">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A25">
-        <v>2</v>
-      </c>
-      <c r="B25">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A26">
-        <v>3</v>
-      </c>
-      <c r="B26">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
+        <v>114</v>
+      </c>
+      <c r="B28">
+        <v>31</v>
+      </c>
+      <c r="C28">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
+        <v>96</v>
+      </c>
+      <c r="B29">
         <v>12</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A27">
-        <v>4</v>
-      </c>
-      <c r="B27">
+      <c r="C29">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A30" t="s">
+        <v>94</v>
+      </c>
+      <c r="B30">
+        <v>25</v>
+      </c>
+      <c r="C30">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A31" t="s">
+        <v>95</v>
+      </c>
+      <c r="B31">
+        <v>23</v>
+      </c>
+      <c r="C31">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A32" t="s">
+        <v>104</v>
+      </c>
+      <c r="B32">
+        <v>229</v>
+      </c>
+      <c r="C32">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A33" t="s">
+        <v>115</v>
+      </c>
+      <c r="B33">
+        <v>14</v>
+      </c>
+      <c r="C33">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A34" t="s">
+        <v>116</v>
+      </c>
+      <c r="B34">
         <v>7</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A28">
-        <v>5</v>
-      </c>
-      <c r="B28">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A29">
-        <v>6</v>
-      </c>
-      <c r="B29">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A30">
-        <v>7</v>
-      </c>
-      <c r="B30">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A31">
+      <c r="C34">
         <v>8</v>
       </c>
-      <c r="B31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A32">
-        <v>9</v>
-      </c>
-      <c r="B32">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A33">
-        <v>11</v>
-      </c>
-      <c r="B33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A34">
-        <v>12</v>
-      </c>
-      <c r="B34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A35">
-        <v>15</v>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A35" t="s">
+        <v>98</v>
       </c>
       <c r="B35">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A36">
-        <v>19</v>
+        <v>78</v>
+      </c>
+      <c r="C35">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A36" t="s">
+        <v>117</v>
       </c>
       <c r="B36">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A37">
+      <c r="C36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A37" t="s">
+        <v>101</v>
+      </c>
+      <c r="B37">
+        <v>9</v>
+      </c>
+      <c r="C37">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A38" t="s">
+        <v>100</v>
+      </c>
+      <c r="B38">
+        <v>10</v>
+      </c>
+      <c r="C38">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A39" t="s">
+        <v>118</v>
+      </c>
+      <c r="B39">
         <v>20</v>
       </c>
-      <c r="B37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A38">
+      <c r="C39">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A40" t="s">
+        <v>119</v>
+      </c>
+      <c r="B40">
+        <v>15</v>
+      </c>
+      <c r="C40">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A41" t="s">
+        <v>120</v>
+      </c>
+      <c r="B41">
+        <v>2036</v>
+      </c>
+      <c r="C41">
+        <v>2811</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A42" t="s">
+        <v>121</v>
+      </c>
+      <c r="B42">
+        <v>12</v>
+      </c>
+      <c r="C42">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A43" t="s">
+        <v>105</v>
+      </c>
+      <c r="B43">
+        <v>31</v>
+      </c>
+      <c r="C43">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A45" s="23"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A46" s="11"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A47" s="8" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A48" s="28" t="s">
+        <v>88</v>
+      </c>
+      <c r="B48" s="28" t="s">
+        <v>90</v>
+      </c>
+      <c r="C48" s="28" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A49" t="s">
+        <v>114</v>
+      </c>
+      <c r="B49">
+        <v>33</v>
+      </c>
+      <c r="C49">
         <v>41</v>
       </c>
-      <c r="B38">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A41" s="23" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A42" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="B42" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A43">
-        <v>1</v>
-      </c>
-      <c r="B43">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A44">
-        <v>2</v>
-      </c>
-      <c r="B44">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A45">
-        <v>3</v>
-      </c>
-      <c r="B45">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A46">
-        <v>4</v>
-      </c>
-      <c r="B46">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A47">
-        <v>5</v>
-      </c>
-      <c r="B47">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A48">
-        <v>6</v>
-      </c>
-      <c r="B48">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A49">
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A50" t="s">
+        <v>96</v>
+      </c>
+      <c r="B50">
+        <v>12</v>
+      </c>
+      <c r="C50">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A51" t="s">
+        <v>94</v>
+      </c>
+      <c r="B51">
+        <v>25</v>
+      </c>
+      <c r="C51">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A52" t="s">
+        <v>95</v>
+      </c>
+      <c r="B52">
+        <v>23</v>
+      </c>
+      <c r="C52">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A53" t="s">
+        <v>104</v>
+      </c>
+      <c r="B53">
+        <v>229</v>
+      </c>
+      <c r="C53">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A54" t="s">
+        <v>115</v>
+      </c>
+      <c r="B54">
+        <v>14</v>
+      </c>
+      <c r="C54">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A55" t="s">
+        <v>116</v>
+      </c>
+      <c r="B55">
         <v>7</v>
       </c>
-      <c r="B49">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A50">
+      <c r="C55">
         <v>8</v>
       </c>
-      <c r="B50">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A51">
-        <v>9</v>
-      </c>
-      <c r="B51">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A52">
-        <v>10</v>
-      </c>
-      <c r="B52">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A53">
-        <v>11</v>
-      </c>
-      <c r="B53">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A54">
-        <v>12</v>
-      </c>
-      <c r="B54">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A55">
-        <v>13</v>
-      </c>
-      <c r="B55">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A56">
-        <v>14</v>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A56" t="s">
+        <v>98</v>
       </c>
       <c r="B56">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A57">
-        <v>15</v>
+        <v>78</v>
+      </c>
+      <c r="C56">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A57" t="s">
+        <v>117</v>
       </c>
       <c r="B57">
         <v>1</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A58">
-        <v>16</v>
+      <c r="C57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A58" t="s">
+        <v>101</v>
       </c>
       <c r="B58">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A59">
-        <v>18</v>
+        <v>9</v>
+      </c>
+      <c r="C58">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A59" t="s">
+        <v>100</v>
       </c>
       <c r="B59">
+        <v>10</v>
+      </c>
+      <c r="C59">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A60" t="s">
+        <v>118</v>
+      </c>
+      <c r="B60">
+        <v>13</v>
+      </c>
+      <c r="C60">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A61" t="s">
+        <v>119</v>
+      </c>
+      <c r="B61">
+        <v>12</v>
+      </c>
+      <c r="C61">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A62" t="s">
+        <v>120</v>
+      </c>
+      <c r="B62">
+        <v>2056</v>
+      </c>
+      <c r="C62">
+        <v>2811</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A63" t="s">
+        <v>121</v>
+      </c>
+      <c r="B63">
+        <v>12</v>
+      </c>
+      <c r="C63">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A64" t="s">
+        <v>105</v>
+      </c>
+      <c r="B64">
+        <v>31</v>
+      </c>
+      <c r="C64">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A68" s="8" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A69" s="28" t="s">
+        <v>88</v>
+      </c>
+      <c r="B69" s="28" t="s">
+        <v>90</v>
+      </c>
+      <c r="C69" s="28" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A70" t="s">
+        <v>114</v>
+      </c>
+      <c r="B70">
+        <v>31</v>
+      </c>
+      <c r="C70">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A71" t="s">
+        <v>96</v>
+      </c>
+      <c r="B71">
+        <v>11</v>
+      </c>
+      <c r="C71">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A72" t="s">
+        <v>94</v>
+      </c>
+      <c r="B72">
+        <v>25</v>
+      </c>
+      <c r="C72">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A73" t="s">
+        <v>95</v>
+      </c>
+      <c r="B73">
+        <v>23</v>
+      </c>
+      <c r="C73">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A74" t="s">
+        <v>104</v>
+      </c>
+      <c r="B74">
+        <v>228</v>
+      </c>
+      <c r="C74">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A75" t="s">
+        <v>115</v>
+      </c>
+      <c r="B75">
+        <v>14</v>
+      </c>
+      <c r="C75">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A76" t="s">
+        <v>116</v>
+      </c>
+      <c r="B76">
+        <v>7</v>
+      </c>
+      <c r="C76">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A77" t="s">
+        <v>98</v>
+      </c>
+      <c r="B77">
+        <v>78</v>
+      </c>
+      <c r="C77">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A78" t="s">
+        <v>117</v>
+      </c>
+      <c r="B78">
         <v>1</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A60">
+      <c r="C78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A79" t="s">
+        <v>101</v>
+      </c>
+      <c r="B79">
+        <v>9</v>
+      </c>
+      <c r="C79">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A80" t="s">
+        <v>100</v>
+      </c>
+      <c r="B80">
+        <v>10</v>
+      </c>
+      <c r="C80">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A81" t="s">
+        <v>118</v>
+      </c>
+      <c r="B81">
         <v>20</v>
       </c>
-      <c r="B60">
+      <c r="C81">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A82" t="s">
+        <v>119</v>
+      </c>
+      <c r="B82">
+        <v>15</v>
+      </c>
+      <c r="C82">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A83" t="s">
+        <v>120</v>
+      </c>
+      <c r="B83">
+        <v>2032</v>
+      </c>
+      <c r="C83">
+        <v>2811</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A84" t="s">
+        <v>121</v>
+      </c>
+      <c r="B84">
+        <v>12</v>
+      </c>
+      <c r="C84">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A85" t="s">
+        <v>105</v>
+      </c>
+      <c r="B85">
+        <v>31</v>
+      </c>
+      <c r="C85">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A89" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A90" s="28" t="s">
+        <v>88</v>
+      </c>
+      <c r="B90" s="28" t="s">
+        <v>90</v>
+      </c>
+      <c r="C90" s="28" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A91" t="s">
+        <v>114</v>
+      </c>
+      <c r="B91">
+        <v>31</v>
+      </c>
+      <c r="C91">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A92" t="s">
+        <v>96</v>
+      </c>
+      <c r="B92">
+        <v>14</v>
+      </c>
+      <c r="C92">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A93" t="s">
+        <v>94</v>
+      </c>
+      <c r="B93">
+        <v>25</v>
+      </c>
+      <c r="C93">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A94" t="s">
+        <v>95</v>
+      </c>
+      <c r="B94">
+        <v>23</v>
+      </c>
+      <c r="C94">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A95" t="s">
+        <v>104</v>
+      </c>
+      <c r="B95">
+        <v>229</v>
+      </c>
+      <c r="C95">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A96" t="s">
+        <v>115</v>
+      </c>
+      <c r="B96">
+        <v>14</v>
+      </c>
+      <c r="C96">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A97" t="s">
+        <v>116</v>
+      </c>
+      <c r="B97">
+        <v>7</v>
+      </c>
+      <c r="C97">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A98" t="s">
+        <v>98</v>
+      </c>
+      <c r="B98">
+        <v>78</v>
+      </c>
+      <c r="C98">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A99" t="s">
+        <v>117</v>
+      </c>
+      <c r="B99">
         <v>1</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A61">
-        <v>23</v>
-      </c>
-      <c r="B61">
+      <c r="C99">
         <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A100" t="s">
+        <v>101</v>
+      </c>
+      <c r="B100">
+        <v>9</v>
+      </c>
+      <c r="C100">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A101" t="s">
+        <v>100</v>
+      </c>
+      <c r="B101">
+        <v>10</v>
+      </c>
+      <c r="C101">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A102" t="s">
+        <v>118</v>
+      </c>
+      <c r="B102">
+        <v>20</v>
+      </c>
+      <c r="C102">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A103" t="s">
+        <v>119</v>
+      </c>
+      <c r="B103">
+        <v>15</v>
+      </c>
+      <c r="C103">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A104" t="s">
+        <v>120</v>
+      </c>
+      <c r="B104">
+        <v>2034</v>
+      </c>
+      <c r="C104">
+        <v>2811</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A105" t="s">
+        <v>121</v>
+      </c>
+      <c r="B105">
+        <v>12</v>
+      </c>
+      <c r="C105">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A106" t="s">
+        <v>105</v>
+      </c>
+      <c r="B106">
+        <v>31</v>
+      </c>
+      <c r="C106">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>